<commit_message>
Updated to fix data input error building 165 MW in all years starting in 2025. Should just be 165 buit in a single year in 2025.
</commit_message>
<xml_diff>
--- a/InputData/elec/BPMCCS/BAU Pol Mandated Cap Const Sched_HK.xlsx
+++ b/InputData/elec/BPMCCS/BAU Pol Mandated Cap Const Sched_HK.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\World Resources Institute\TRAC City - HK 2050 is now\EPS HK 2.0\eps-2.0.0-us-wipF\InputData\elec\BPMCCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\Hong Kong\Models\eps-hongkong\InputData\elec\BPMCCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_992A8050BFE2D6DF8CCA274F53859F76552817E4" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B2E0ED95-5300-4357-8513-3028F7428BA5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="MSD" sheetId="7" r:id="rId4"/>
     <sheet name="BPMCCS" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,12 +31,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>微软用户</author>
   </authors>
   <commentList>
-    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="E8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="C14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="C15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -115,7 +114,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="G31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -141,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G56" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="G56" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -167,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G82" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="G82" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -193,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G107" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="G107" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -224,12 +223,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>微软用户</author>
   </authors>
   <commentList>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="C10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -255,7 +254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="E13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -281,7 +280,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
+    <comment ref="D25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -307,7 +306,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
+    <comment ref="D26" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -333,7 +332,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
+    <comment ref="D28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1486,7 +1485,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="20">
     <font>
       <sz val="11"/>
@@ -2660,7 +2659,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2813,7 +2812,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5477,7 +5476,7 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I23" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="I23" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -5486,7 +5485,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView zoomScale="92" workbookViewId="0">
@@ -5901,7 +5900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{806D35C6-EE1D-45D7-BD9C-624FB3BAF2E4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -5932,17 +5931,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AK17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB23" sqref="AB23"/>
+      <selection pane="bottomRight" activeCell="M17" sqref="M17:AK17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7800,79 +7799,79 @@
         <v>165</v>
       </c>
       <c r="M17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="N17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="O17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="P17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="Q17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="R17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="S17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="T17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="U17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="V17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="W17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="X17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="Y17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="Z17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="AA17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="AB17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="AC17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="AD17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="AE17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="AF17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="AG17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="AH17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="AI17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="AJ17">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="AK17">
-        <v>165</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7891,15 +7890,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095990DC6317597479C114DD4E6AB1F33" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="00c0eb7d4c43453177323eb1ac58d7e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="7889d872-e2a2-4afb-87bc-97561eced75f" xmlns:ns3="c9df191c-55f2-496b-9838-9a5abe4742ad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5fe72540fcc493259a136614ad94e00" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -8133,6 +8123,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E08065FD-5B6D-42CE-B8BF-76B07783FA76}">
   <ds:schemaRefs>
@@ -8152,14 +8151,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A9C258F-8B2D-4324-9C14-B134F59C77B8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E515567C-76CC-4E3A-8CA7-857A9CB73A2D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8177,4 +8168,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A9C258F-8B2D-4324-9C14-B134F59C77B8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>